<commit_message>
Expanded RulesGrid in JSON string
</commit_message>
<xml_diff>
--- a/Project KitchenBook.xlsx
+++ b/Project KitchenBook.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raj\GitHub\Repos\ra-innovations\WebApp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926F12C5-AEF6-4F2D-AD94-D1248468877B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86254142-103A-44CF-8D76-3018BF16B685}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Objects" sheetId="1" r:id="rId1"/>
     <sheet name="Use Case" sheetId="2" r:id="rId2"/>
     <sheet name="Commands" sheetId="3" r:id="rId3"/>
+    <sheet name="CommandRulesTable" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1551895832" val="944" rev="123" revOS="4"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="200">
   <si>
     <t>Data Blocks</t>
   </si>
@@ -266,9 +267,6 @@
     <t>"Tools"</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Main Page</t>
   </si>
   <si>
@@ -453,6 +451,186 @@
   </si>
   <si>
     <t>Repeat Add comment</t>
+  </si>
+  <si>
+    <t>Reads title &amp; Summary</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>CommenterID</t>
+  </si>
+  <si>
+    <t>Defaults to 0 (implies recipe comment)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>CommentID</t>
+  </si>
+  <si>
+    <t>StepNumber</t>
+  </si>
+  <si>
+    <t>Step # done</t>
+  </si>
+  <si>
+    <t>Stop snoozing any timers</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>RECIPE</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>(onPlayRecipeName, onPlayRecipeDescription, onListIngredients, onListToolsNeeded)</t>
+  </si>
+  <si>
+    <t>(Before steps start)</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>INGREDIENTS</t>
+  </si>
+  <si>
+    <t>onListIngredients</t>
+  </si>
+  <si>
+    <t>(Functions lists ingredients, creates list of missing ingredients, recommends substitutes)</t>
+  </si>
+  <si>
+    <t>TOOLS</t>
+  </si>
+  <si>
+    <t>onListToolsNeeded</t>
+  </si>
+  <si>
+    <t>LIST STEPS</t>
+  </si>
+  <si>
+    <t>onListSteps</t>
+  </si>
+  <si>
+    <t>ADD COMMENT</t>
+  </si>
+  <si>
+    <t>onAddComment</t>
+  </si>
+  <si>
+    <t>READ COMMENTS</t>
+  </si>
+  <si>
+    <t>onReadComments</t>
+  </si>
+  <si>
+    <t>(Does not pause step timers. Pauses video &amp; audio)</t>
+  </si>
+  <si>
+    <t>STEPS</t>
+  </si>
+  <si>
+    <t>PAUSE</t>
+  </si>
+  <si>
+    <t>onPauseRecipe</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>onContinueRecipe</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>onStopRecipe</t>
+  </si>
+  <si>
+    <t>SKIP STEP</t>
+  </si>
+  <si>
+    <t>onSkipStep</t>
+  </si>
+  <si>
+    <t>onListTools</t>
+  </si>
+  <si>
+    <t>RESTART STEP</t>
+  </si>
+  <si>
+    <t>onStartStep</t>
+  </si>
+  <si>
+    <t>MISCELLANEOUS</t>
+  </si>
+  <si>
+    <t>SUBSTITUTE</t>
+  </si>
+  <si>
+    <t>onIngredientSubstitute</t>
+  </si>
+  <si>
+    <t>CONVERT</t>
+  </si>
+  <si>
+    <t>onUnitConverstion</t>
+  </si>
+  <si>
+    <t>START TIMER</t>
+  </si>
+  <si>
+    <t>onStartTimer</t>
+  </si>
+  <si>
+    <t>CANCEL TIMER</t>
+  </si>
+  <si>
+    <t>onCancelTimer</t>
+  </si>
+  <si>
+    <t>END TIMER</t>
+  </si>
+  <si>
+    <t>onEndTimer</t>
+  </si>
+  <si>
+    <t>LIST TIMERS</t>
+  </si>
+  <si>
+    <t>onListTimers</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>onAnnounceTitle</t>
+  </si>
+  <si>
+    <t>onAnnounceDescription</t>
+  </si>
+  <si>
+    <t>onStartRecipe()</t>
+  </si>
+  <si>
+    <t>onAnnounceTitle()</t>
+  </si>
+  <si>
+    <t>onAnnounceDescription()</t>
   </si>
 </sst>
 </file>
@@ -937,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1027,6 +1205,8 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1378,15 +1558,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1011"/>
+  <dimension ref="A1:AB1013"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
@@ -1679,26 +1859,24 @@
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-      <c r="C25" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>13</v>
-      </c>
+    <row r="25" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="14"/>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
       <c r="C26" s="13" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>13</v>
@@ -1708,29 +1886,29 @@
     <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
       <c r="C27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="14"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
       <c r="C28" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="14"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
       <c r="C29" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>21</v>
@@ -1743,7 +1921,7 @@
     <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
       <c r="C30" s="13" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>21</v>
@@ -1756,10 +1934,10 @@
     <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
       <c r="C31" s="13" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>13</v>
@@ -1769,10 +1947,10 @@
     <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
       <c r="C32" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>13</v>
@@ -1782,7 +1960,7 @@
     <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
       <c r="C33" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>21</v>
@@ -1795,7 +1973,7 @@
     <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
       <c r="C34" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>21</v>
@@ -1808,7 +1986,7 @@
     <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
       <c r="C35" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>21</v>
@@ -1820,9 +1998,15 @@
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="C36" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="F36" s="14"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1833,27 +2017,21 @@
       <c r="F37" s="14"/>
     </row>
     <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="15"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D39" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="14"/>
-      <c r="C39" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>10</v>
@@ -1863,30 +2041,36 @@
     <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="14"/>
       <c r="C40" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="14"/>
+      <c r="C41" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D41" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E41" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="15"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
       <c r="F41" s="14"/>
     </row>
-    <row r="42" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15"/>
-      <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="15"/>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -1894,52 +2078,72 @@
       <c r="F43" s="14"/>
     </row>
     <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="14"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="15"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="B45" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
     </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="15"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+    <row r="46" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="69"/>
+      <c r="C46" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="14"/>
       <c r="F46" s="14"/>
     </row>
     <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="15"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="F47" s="14"/>
     </row>
     <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="15"/>
-      <c r="C48" s="13"/>
+      <c r="C48" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="14"/>
     </row>
     <row r="49" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="15"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="C49" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="14"/>
     </row>
     <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="15"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="14"/>
     </row>
     <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8668,6 +8872,20 @@
       <c r="D1011" s="14"/>
       <c r="E1011" s="14"/>
       <c r="F1011" s="14"/>
+    </row>
+    <row r="1012" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1012" s="15"/>
+      <c r="C1012" s="14"/>
+      <c r="D1012" s="14"/>
+      <c r="E1012" s="14"/>
+      <c r="F1012" s="14"/>
+    </row>
+    <row r="1013" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1013" s="15"/>
+      <c r="C1013" s="14"/>
+      <c r="D1013" s="14"/>
+      <c r="E1013" s="14"/>
+      <c r="F1013" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.39374999999999999" footer="0.39374999999999999"/>
@@ -11884,11 +12102,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360F7479-26F6-42CB-8830-81A74C2CE1C6}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1035" topLeftCell="A24" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11897,7 +12115,7 @@
     <col min="2" max="2" width="12.42578125" style="24" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="25"/>
-    <col min="5" max="5" width="10" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="26" customWidth="1"/>
     <col min="6" max="6" width="16" style="53" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.140625" style="54"/>
     <col min="9" max="9" width="9.140625" style="55"/>
@@ -11910,22 +12128,22 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1" s="32" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
       <c r="E1" s="34"/>
       <c r="F1" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
       <c r="I1" s="37"/>
       <c r="J1" s="68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L1" s="57"/>
       <c r="M1" s="57"/>
@@ -11958,9 +12176,7 @@
       <c r="N3" s="64"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
-        <v>79</v>
-      </c>
+      <c r="B4" s="28"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="30"/>
@@ -11974,321 +12190,342 @@
       <c r="M4" s="66"/>
       <c r="N4" s="67"/>
     </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C7" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F8" s="53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F9" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F10" s="53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F12" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F14" s="53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="J15" s="27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="J13" s="27" t="s">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G16" s="54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G14" s="54" t="s">
+      <c r="K16" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="59" t="s">
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F18" s="53" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F16" s="53" t="s">
+      <c r="J18" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="27" t="s">
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G19" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="59" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G17" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" s="59" t="s">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F21" s="53" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="53" t="s">
+      <c r="J21" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="27" t="s">
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G22" s="54" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G20" s="54" t="s">
+      <c r="J22" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="K22" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="59" t="s">
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F24" s="53" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F22" s="53" t="s">
+      <c r="J24" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="27" t="s">
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G25" s="54" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G23" s="54" t="s">
+      <c r="J25" s="27" t="s">
         <v>102</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="J25" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="K25" s="59" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.2">
       <c r="F27" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27" s="59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F29" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="J29" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="27" t="s">
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G30" s="54" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G28" s="54" t="s">
+      <c r="J30" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="J28" s="27" t="s">
+      <c r="K30" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="K28" s="59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E30" s="26" t="s">
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="26" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F31" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="K31" s="59" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.2">
       <c r="F33" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="J33" s="27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K33" s="59" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="J34" s="27" t="s">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="F35" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="K35" s="59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="J36" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="K36" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="K34" s="59" t="s">
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="J37" s="27" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="J35" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="G36" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="K36" s="59" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.2">
       <c r="G38" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" s="59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="G40" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" s="59" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D42" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="J42" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="J43" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="G44" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K44" s="59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="J46" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="G47" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F51" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="J51" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F53" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="J53" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F54" s="53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F56" s="53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F58" s="53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F59" s="53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F63" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="J63" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="G64" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="J64" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="K64" s="59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E66" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F67" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="K67" s="59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F69" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="J69" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="J70" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="K70" s="59" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="J71" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G72" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="K72" s="59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G74" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K74" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="K38" s="59" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="J40" s="27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="J41" s="27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="G42" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="K42" s="59" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="J44" s="27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="G45" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="K45" s="59" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F49" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="J49" s="27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F51" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="J51" s="27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F52" s="53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F54" s="53" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F56" s="53" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F57" s="53" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F61" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="J61" s="27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G62" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="J62" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="K62" s="59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E64" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="65" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F65" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="K65" s="59" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="67" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F67" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="J67" s="27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="J68" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="K68" s="59" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="J69" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G70" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="K70" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="72" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G72" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="K72" s="59" t="s">
-        <v>139</v>
+    </row>
+    <row r="77" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F77" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="K77" s="59" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -12300,4 +12537,367 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEC74E-5A4C-4548-96C8-49DE44A05ECC}">
+  <dimension ref="B1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="70"/>
+    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="70">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="70">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C5" s="70">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="70">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="70">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="70">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="70">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="70">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C11" s="70">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="70">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="70">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="70">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="70">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="70">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="70">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="70">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="70">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="70">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="70">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="70">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="70">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" s="70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="70">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="70">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="70">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="70">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="70">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="70">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>